<commit_message>
Regenerate BOMs from bomtool
</commit_message>
<xml_diff>
--- a/quote-pack/motor/motor-bom.xlsx
+++ b/quote-pack/motor/motor-bom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="200">
   <si>
     <t>Line no in motor-v4 BOM</t>
   </si>
@@ -196,18 +196,27 @@
     <t>sr-cn-camcon2w</t>
   </si>
   <si>
+    <t>rapid</t>
+  </si>
+  <si>
+    <t>21-2448</t>
+  </si>
+  <si>
+    <t>Pluggable terminal block 2way 7.5mm pitch male horiz</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>low stock (want 158, while only 237 are available)</t>
+  </si>
+  <si>
+    <t>sr-cn-camcon2w-5mm</t>
+  </si>
+  <si>
     <t>farnell</t>
   </si>
   <si>
-    <t>Pluggable terminal block 2way 7.5mm pitch male horiz</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>sr-cn-camcon2w-5mm</t>
-  </si>
-  <si>
     <t>Pluggable terminal block 2way 5mm pitch male horiz</t>
   </si>
   <si>
@@ -295,9 +304,6 @@
     <t>sr-d-gsot05c</t>
   </si>
   <si>
-    <t>78-GSOT05C-E3-08</t>
-  </si>
-  <si>
     <t>5V unidirectional dual TVS diode 480W common anode</t>
   </si>
   <si>
@@ -307,7 +313,7 @@
     <t>sr-d-gsot24c</t>
   </si>
   <si>
-    <t>78-GSOT24C-E3-08</t>
+    <t>511-ESDA25LY</t>
   </si>
   <si>
     <t>24V unidirectional dual TVS diode 325W common anode</t>
@@ -362,6 +368,9 @@
   </si>
   <si>
     <t>F1</t>
+  </si>
+  <si>
+    <t>awaiting delivery</t>
   </si>
   <si>
     <t>sr-ic-adum3211arz</t>
@@ -1079,17 +1088,20 @@
       <c r="C18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="2">
-        <v>3882391.0</v>
+      <c r="D18" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="E18" s="2">
         <v>1.0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19">
@@ -1097,10 +1109,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D19" s="2">
         <v>3882093.0</v>
@@ -1109,10 +1121,10 @@
         <v>2.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20">
@@ -1120,22 +1132,22 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D20" s="2">
-        <v>1593441.0</v>
+        <v>1022233.0</v>
       </c>
       <c r="E20" s="2">
         <v>1.0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21">
@@ -1143,10 +1155,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D21" s="2">
         <v>1577743.0</v>
@@ -1155,10 +1167,10 @@
         <v>1.0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22">
@@ -1166,10 +1178,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D22" s="2">
         <v>1717073.0</v>
@@ -1178,10 +1190,10 @@
         <v>1.0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23">
@@ -1189,10 +1201,10 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D23" s="2">
         <v>2490660.0</v>
@@ -1201,10 +1213,10 @@
         <v>1.0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24">
@@ -1212,10 +1224,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D24" s="2">
         <v>1825875.0</v>
@@ -1224,10 +1236,10 @@
         <v>1.0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25">
@@ -1235,10 +1247,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D25" s="2">
         <v>1081204.0</v>
@@ -1247,10 +1259,10 @@
         <v>1.0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26">
@@ -1258,10 +1270,10 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D26" s="2">
         <v>1081205.0</v>
@@ -1270,10 +1282,10 @@
         <v>2.0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27">
@@ -1281,10 +1293,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D27" s="2">
         <v>1081206.0</v>
@@ -1293,10 +1305,10 @@
         <v>5.0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28">
@@ -1304,10 +1316,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D28" s="2">
         <v>8735646.0</v>
@@ -1316,10 +1328,10 @@
         <v>1.0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29">
@@ -1327,22 +1339,22 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>94</v>
+        <v>67</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2433345.0</v>
       </c>
       <c r="E29" s="2">
         <v>1.0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30">
@@ -1350,22 +1362,22 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E30" s="2">
         <v>2.0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31">
@@ -1373,10 +1385,10 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D31" s="2">
         <v>1459121.0</v>
@@ -1385,10 +1397,10 @@
         <v>1.0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32">
@@ -1396,10 +1408,10 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D32" s="2">
         <v>9802789.0</v>
@@ -1408,10 +1420,10 @@
         <v>1.0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33">
@@ -1419,10 +1431,10 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D33" s="2">
         <v>1669673.0</v>
@@ -1431,10 +1443,10 @@
         <v>10.0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34">
@@ -1442,10 +1454,10 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D34" s="2">
         <v>2580009.0</v>
@@ -1454,10 +1466,10 @@
         <v>1.0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35">
@@ -1465,22 +1477,25 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E35" s="2">
         <v>1.0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="36">
@@ -1488,22 +1503,22 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E36" s="2">
         <v>1.0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37">
@@ -1511,10 +1526,10 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D37" s="2">
         <v>1146033.0</v>
@@ -1523,10 +1538,10 @@
         <v>1.0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38">
@@ -1534,22 +1549,22 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E38" s="2">
         <v>1.0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39">
@@ -1557,10 +1572,10 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D39" s="2">
         <v>1838508.0</v>
@@ -1569,10 +1584,10 @@
         <v>1.0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40">
@@ -1580,22 +1595,22 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E40" s="2">
         <v>2.0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41">
@@ -1603,10 +1618,10 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D41" s="2">
         <v>2061657.0</v>
@@ -1615,10 +1630,10 @@
         <v>1.0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42">
@@ -1626,10 +1641,10 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D42" s="2">
         <v>2217974.0</v>
@@ -1638,10 +1653,10 @@
         <v>2.0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43">
@@ -1649,10 +1664,10 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D43" s="2">
         <v>1318243.0</v>
@@ -1661,10 +1676,10 @@
         <v>1.0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44">
@@ -1672,10 +1687,10 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D44" s="2">
         <v>8529949.0</v>
@@ -1684,10 +1699,10 @@
         <v>3.0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45">
@@ -1695,10 +1710,10 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D45" s="2">
         <v>1686083.0</v>
@@ -1707,10 +1722,10 @@
         <v>2.0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46">
@@ -1718,22 +1733,22 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E46" s="2">
         <v>1.0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47">
@@ -1741,10 +1756,10 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D47" s="2">
         <v>1081229.0</v>
@@ -1753,10 +1768,10 @@
         <v>2.0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48">
@@ -1764,7 +1779,7 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>9</v>
@@ -1776,10 +1791,10 @@
         <v>1.0</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49">
@@ -1787,7 +1802,7 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>9</v>
@@ -1799,10 +1814,10 @@
         <v>1.0</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50">
@@ -1810,7 +1825,7 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>9</v>
@@ -1822,10 +1837,10 @@
         <v>2.0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51">
@@ -1833,7 +1848,7 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>9</v>
@@ -1845,10 +1860,10 @@
         <v>14.0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52">
@@ -1856,7 +1871,7 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>9</v>
@@ -1868,10 +1883,10 @@
         <v>10.0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53">
@@ -1879,7 +1894,7 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>9</v>
@@ -1891,10 +1906,10 @@
         <v>3.0</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54">
@@ -1902,7 +1917,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>9</v>
@@ -1914,10 +1929,10 @@
         <v>7.0</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55">
@@ -1925,7 +1940,7 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>9</v>
@@ -1937,10 +1952,10 @@
         <v>6.0</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56">
@@ -1948,7 +1963,7 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>9</v>
@@ -1960,10 +1975,10 @@
         <v>1.0</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57">
@@ -1971,7 +1986,7 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>9</v>
@@ -1983,10 +1998,10 @@
         <v>5.0</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58">
@@ -1994,7 +2009,7 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>9</v>
@@ -2006,10 +2021,10 @@
         <v>7.0</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59">
@@ -2017,10 +2032,10 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D59" s="2">
         <v>1555987.0</v>
@@ -2029,10 +2044,10 @@
         <v>1.0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60">
@@ -2040,10 +2055,10 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D60" s="2">
         <v>1611803.0</v>
@@ -2052,10 +2067,10 @@
         <v>1.0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61">

</xml_diff>